<commit_message>
Adición de calculos abundancia Fitoplancton
</commit_message>
<xml_diff>
--- a/03_An_Expl_DatosBiologicos/Biologicos/DatosP_Fitoplancton/Event_ID_EXP.PACiFICO_2021.xlsx
+++ b/03_An_Expl_DatosBiologicos/Biologicos/DatosP_Fitoplancton/Event_ID_EXP.PACiFICO_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Ictioplancton\Analisis_Exp_Pac\Ictioplancton_ExPacifico2021\01_Analisis_Exploratorio\02_Datos\Biologicos\DatosP_Fitoplancton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Expedición Pacífico\Ictioplancton_ExPacifico2021\03_An_Expl_DatosBiologicos\Biologicos\DatosP_Fitoplancton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFD740C-ECA5-4C68-BAB8-E6B01B2E09F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0643A2-1DE9-4B65-96DA-40AC455A58B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="2" r:id="rId1"/>
@@ -972,50 +972,49 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="27" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="27" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1025,30 +1024,33 @@
     <xf numFmtId="167" fontId="27" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="26" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="23" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1142,7 +1144,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Datos_Evento_Muestreo"/>
@@ -5935,15 +5937,15 @@
   <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30:XFD30"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -6161,66 +6163,66 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="9">
+      <c r="B4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="30">
         <v>44315</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="21">
         <v>0.69444444444444453</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="E4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="15" t="str">
+      <c r="I4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="24" t="str">
         <f>INDEX([1]Datos_Evento_Muestreo!$L$2:$L$37,MATCH(D4,[1]Datos_Evento_Muestreo!$J$2:$J$37,0))</f>
         <v>S06A</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="10" t="s">
+      <c r="M4" s="25"/>
+      <c r="N4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="11">
+      <c r="S4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="27">
         <v>2</v>
       </c>
-      <c r="U4" s="11">
+      <c r="U4" s="27">
         <v>-78.11</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="V4" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -7799,17 +7801,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="21">
+      <c r="C30" s="20">
         <v>44320</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="21">
         <v>0.4069444444444445</v>
       </c>
       <c r="E30" s="14" t="s">
@@ -7821,44 +7823,44 @@
       <c r="G30" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="H30" s="22" t="s">
         <v>29</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="24" t="s">
+      <c r="J30" s="23" t="s">
         <v>22</v>
       </c>
       <c r="K30" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="L30" s="25" t="str">
+      <c r="L30" s="24" t="str">
         <f>INDEX([1]Datos_Evento_Muestreo!$L$2:$L$37,MATCH(D30,[1]Datos_Evento_Muestreo!$J$2:$J$37,0))</f>
         <v>S02A</v>
       </c>
-      <c r="M30" s="26"/>
+      <c r="M30" s="25"/>
       <c r="N30" s="14" t="s">
         <v>24</v>
       </c>
       <c r="O30" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="27" t="s">
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="26" t="s">
         <v>88</v>
       </c>
       <c r="S30" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="T30" s="28">
+      <c r="T30" s="27">
         <v>2.8</v>
       </c>
-      <c r="U30" s="28">
+      <c r="U30" s="27">
         <v>-78.11</v>
       </c>
-      <c r="V30" s="29" t="s">
+      <c r="V30" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -8400,7 +8402,7 @@
       <c r="C2" s="9">
         <v>44315</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="17">
         <v>0.43958333333333338</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -8460,7 +8462,7 @@
       <c r="C3" s="9">
         <v>44315</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="18">
         <v>0.47083333333333338</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -8520,7 +8522,7 @@
       <c r="C4" s="9">
         <v>44315</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>0.68263888888888891</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -8580,7 +8582,7 @@
       <c r="C5" s="9">
         <v>44315</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>0.71458333333333324</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -8640,7 +8642,7 @@
       <c r="C6" s="9">
         <v>44316</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>0.27638888888888885</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -8700,7 +8702,7 @@
       <c r="C7" s="9">
         <v>44316</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>0.2951388888888889</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -8760,7 +8762,7 @@
       <c r="C8" s="9">
         <v>44316</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>0.4993055555555555</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -8820,7 +8822,7 @@
       <c r="C9" s="9">
         <v>44316</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>0.52777777777777779</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -8880,7 +8882,7 @@
       <c r="C10" s="12">
         <v>44317</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>0.27916666666666667</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -8940,7 +8942,7 @@
       <c r="C11" s="12">
         <v>44317</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>0.29791666666666666</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -9000,7 +9002,7 @@
       <c r="C12" s="12">
         <v>44317</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>7.33</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -9060,7 +9062,7 @@
       <c r="C13" s="12">
         <v>44317</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>0.53749999999999998</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -10380,7 +10382,7 @@
       <c r="C35" s="12">
         <v>44320</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="19">
         <v>0.6694444444444444</v>
       </c>
       <c r="E35" s="2" t="s">

</xml_diff>